<commit_message>
Đăng ký đề tài nhóm TUấn thành + Minh Tuấn, Tang Wen Miao Jin + Nguyễn Xuân Hồng
</commit_message>
<xml_diff>
--- a/document/ToolAsign.xlsx
+++ b/document/ToolAsign.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20363"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A330695-F207-4EEE-B877-675C4C43992E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC83817-34AE-4B81-B8BD-DEF7BB297E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3390" yWindow="3390" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t>Bùi Công Minh+ Nguyễn Kim Khôi</t>
+  </si>
+  <si>
+    <t>Phạm Minh Tuấn + Nguyễn Tuấn Thành</t>
+  </si>
+  <si>
+    <t>Tang Wen Miao Jin + Nguyễn Xuân Hồng</t>
   </si>
 </sst>
 </file>
@@ -387,16 +393,16 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="128.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="128.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -404,7 +410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -412,7 +418,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -420,17 +426,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -438,7 +447,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>

</xml_diff>